<commit_message>
Fix the population creation function. Now one class cant have two lessons at the same time
</commit_message>
<xml_diff>
--- a/test/uch_plan_85.xlsx
+++ b/test/uch_plan_85.xlsx
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C515"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>